<commit_message>
label change for FMI
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_LISA_P2.xlsx
+++ b/rmonize/data_dictionary/DD_LISA_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F818021-E49C-40A7-B0FC-EA3EFE76F08F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02189822-0A78-4882-91DE-477A791CE83C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>LDL cholesterol intake</t>
   </si>
   <si>
-    <t xml:space="preserve"> HDL_15 </t>
-  </si>
-  <si>
     <t>HDL cholesterol [mmol/L]</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
   </si>
   <si>
     <t>UB_fmi_15</t>
-  </si>
-  <si>
-    <t>Calculated from BIA measurement at age 15</t>
   </si>
   <si>
     <t>UB_fbm_15</t>
@@ -605,6 +599,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL_15 </t>
+  </si>
+  <si>
+    <t>FMI [kg/ m2] calculated from BIA measurement at age 15</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -1214,7 +1214,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
@@ -1228,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>22</v>
@@ -1242,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>23</v>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>24</v>
@@ -1270,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>25</v>
@@ -1284,7 +1284,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>26</v>
@@ -1372,10 +1372,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>10</v>
@@ -1386,10 +1386,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>5</v>
@@ -1400,10 +1400,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>10</v>
@@ -1414,10 +1414,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>5</v>
@@ -1429,10 +1429,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>5</v>
@@ -1443,10 +1443,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>10</v>
@@ -1457,10 +1457,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>10</v>
@@ -1471,10 +1471,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>52</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>10</v>
@@ -1485,10 +1485,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>10</v>
@@ -1500,10 +1500,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>10</v>
@@ -1514,10 +1514,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>10</v>
@@ -1528,10 +1528,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>10</v>
@@ -1542,10 +1542,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>10</v>
@@ -1556,10 +1556,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>10</v>
@@ -1570,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>10</v>
@@ -1584,10 +1584,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>10</v>
@@ -1598,10 +1598,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>10</v>
@@ -1612,10 +1612,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>10</v>
@@ -1626,10 +1626,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>10</v>
@@ -1640,10 +1640,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>10</v>
@@ -1654,10 +1654,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>10</v>
@@ -1668,10 +1668,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>10</v>
@@ -1682,10 +1682,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>10</v>
@@ -1696,10 +1696,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>10</v>
@@ -1710,10 +1710,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>10</v>
@@ -1724,10 +1724,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>10</v>
@@ -1738,10 +1738,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>10</v>
@@ -1755,10 +1755,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>10</v>
@@ -1772,10 +1772,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>10</v>
@@ -1786,10 +1786,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>10</v>
@@ -1800,10 +1800,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>10</v>
@@ -1814,10 +1814,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>10</v>
@@ -1828,10 +1828,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>10</v>
@@ -1842,10 +1842,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>10</v>
@@ -1856,10 +1856,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>10</v>
@@ -1870,10 +1870,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>10</v>
@@ -1885,10 +1885,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>10</v>
@@ -1899,10 +1899,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>10</v>
@@ -1913,10 +1913,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>10</v>
@@ -1930,10 +1930,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>10</v>
@@ -1947,10 +1947,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>10</v>
@@ -1964,10 +1964,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>10</v>
@@ -1981,10 +1981,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>10</v>
@@ -1998,10 +1998,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>10</v>
@@ -2015,10 +2015,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>10</v>
@@ -2032,10 +2032,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>10</v>
@@ -2049,10 +2049,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>10</v>
@@ -2066,10 +2066,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>10</v>
@@ -2083,10 +2083,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>10</v>
@@ -2101,10 +2101,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>10</v>
@@ -2118,10 +2118,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>10</v>
@@ -2135,10 +2135,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>10</v>
@@ -2152,10 +2152,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>10</v>
@@ -2169,10 +2169,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>10</v>
@@ -2186,10 +2186,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>10</v>
@@ -2200,10 +2200,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>10</v>
@@ -2217,10 +2217,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>10</v>
@@ -2231,10 +2231,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>10</v>
@@ -2454,7 +2454,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2463,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2475,7 +2475,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2618,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2739,7 +2739,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2772,7 +2772,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2783,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2849,117 +2849,117 @@
         <v>2</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B37" s="17">
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B39" s="17">
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B40" s="17">
         <v>3</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="17">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="17">
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="17">
         <v>3</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="17">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="17">
         <v>2</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="17">
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2977,6 +2977,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3217,18 +3229,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -3238,6 +3238,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A35BFFB-6462-4C07-9656-4D34A1531B24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3254,15 +3265,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated LISA P2 DD, DPE (+DATA) to update label for LDLC_15. Updated variable name + label for FFQGI_15 and FFQGL_15.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_LISA_P2.xlsx
+++ b/rmonize/data_dictionary/DD_LISA_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02189822-0A78-4882-91DE-477A791CE83C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5690281B-013C-4C48-9F4A-DB505DF55E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t xml:space="preserve">LDLC_15 </t>
   </si>
   <si>
-    <t>LDL cholesterol intake</t>
-  </si>
-  <si>
     <t>HDL cholesterol [mmol/L]</t>
   </si>
   <si>
@@ -274,18 +271,6 @@
     <t>Fructose (fruit sugar) (mg)</t>
   </si>
   <si>
-    <t>FFQ_GI_15</t>
-  </si>
-  <si>
-    <t>glycaemic index</t>
-  </si>
-  <si>
-    <t>FFQ_GL_15</t>
-  </si>
-  <si>
-    <t>glycaemic load</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQMNA_15 </t>
   </si>
   <si>
@@ -605,6 +590,21 @@
   </si>
   <si>
     <t>FMI [kg/ m2] calculated from BIA measurement at age 15</t>
+  </si>
+  <si>
+    <t>FFQGL_15</t>
+  </si>
+  <si>
+    <t>FFQGI_15</t>
+  </si>
+  <si>
+    <t>Glycemic Load calculated from FFQ data</t>
+  </si>
+  <si>
+    <t>Glycemic Index calculated from FFQ data</t>
+  </si>
+  <si>
+    <t>LDL cholesterol [mmol/L]</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -1214,7 +1214,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
@@ -1228,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>22</v>
@@ -1242,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>23</v>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>24</v>
@@ -1270,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>25</v>
@@ -1284,7 +1284,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>26</v>
@@ -1361,7 +1361,7 @@
         <v>35</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>10</v>
@@ -1372,10 +1372,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>10</v>
@@ -1386,10 +1386,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>5</v>
@@ -1400,10 +1400,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>10</v>
@@ -1414,10 +1414,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>5</v>
@@ -1429,10 +1429,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>5</v>
@@ -1443,10 +1443,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>10</v>
@@ -1457,10 +1457,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>10</v>
@@ -1471,10 +1471,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>10</v>
@@ -1485,10 +1485,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>10</v>
@@ -1500,10 +1500,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>10</v>
@@ -1514,10 +1514,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>10</v>
@@ -1528,10 +1528,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>10</v>
@@ -1542,10 +1542,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>10</v>
@@ -1556,10 +1556,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>10</v>
@@ -1570,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>10</v>
@@ -1584,10 +1584,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>10</v>
@@ -1598,10 +1598,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>10</v>
@@ -1612,10 +1612,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>10</v>
@@ -1626,10 +1626,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>10</v>
@@ -1640,10 +1640,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>10</v>
@@ -1654,10 +1654,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>10</v>
@@ -1668,38 +1668,38 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="D42" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>10</v>
@@ -1710,10 +1710,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>10</v>
@@ -1724,10 +1724,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>10</v>
@@ -1738,10 +1738,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>10</v>
@@ -1755,10 +1755,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>10</v>
@@ -1772,10 +1772,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>10</v>
@@ -1786,10 +1786,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>10</v>
@@ -1800,10 +1800,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>10</v>
@@ -1814,10 +1814,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>10</v>
@@ -1828,10 +1828,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>10</v>
@@ -1842,10 +1842,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>10</v>
@@ -1856,10 +1856,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>10</v>
@@ -1870,10 +1870,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>10</v>
@@ -1885,10 +1885,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>10</v>
@@ -1899,10 +1899,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>10</v>
@@ -1913,10 +1913,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>10</v>
@@ -1930,10 +1930,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>10</v>
@@ -1947,10 +1947,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>10</v>
@@ -1964,10 +1964,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>10</v>
@@ -1981,10 +1981,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>10</v>
@@ -1998,10 +1998,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>10</v>
@@ -2015,10 +2015,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>10</v>
@@ -2032,10 +2032,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>10</v>
@@ -2049,10 +2049,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>10</v>
@@ -2066,10 +2066,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>10</v>
@@ -2083,10 +2083,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>10</v>
@@ -2101,10 +2101,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>10</v>
@@ -2118,10 +2118,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>10</v>
@@ -2135,10 +2135,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>10</v>
@@ -2152,10 +2152,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>10</v>
@@ -2169,10 +2169,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>10</v>
@@ -2186,10 +2186,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>10</v>
@@ -2200,10 +2200,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>10</v>
@@ -2217,10 +2217,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>10</v>
@@ -2231,10 +2231,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>10</v>
@@ -2454,7 +2454,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2463,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2475,7 +2475,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2618,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2739,7 +2739,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2772,7 +2772,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2783,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2849,117 +2849,117 @@
         <v>2</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B37" s="17">
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B39" s="17">
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B40" s="17">
         <v>3</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="17">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="17">
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="17">
         <v>3</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="17">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="17">
         <v>2</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="17">
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2968,15 +2968,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -2986,6 +2977,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3230,20 +3230,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GL-4 DD_LISA_P2 small update to match P1
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_LISA_P2.xlsx
+++ b/rmonize/data_dictionary/DD_LISA_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5690281B-013C-4C48-9F4A-DB505DF55E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CB1C8-81AB-4699-BB43-465BC78BC798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11025" yWindow="0" windowWidth="11025" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="192">
   <si>
     <t>index</t>
   </si>
@@ -605,6 +605,12 @@
   </si>
   <si>
     <t>LDL cholesterol [mmol/L]</t>
+  </si>
+  <si>
+    <t>General or specialist university entrance qualification</t>
+  </si>
+  <si>
+    <t>Other degree</t>
   </si>
 </sst>
 </file>
@@ -772,9 +778,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -812,7 +818,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -918,7 +924,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1060,7 +1066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1070,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -2442,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2558,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2980,15 +2986,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3229,6 +3226,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
@@ -3241,14 +3247,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A35BFFB-6462-4C07-9656-4D34A1531B24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3265,4 +3263,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>